<commit_message>
Fixed unit issue on DPIE data
</commit_message>
<xml_diff>
--- a/matlab/Data_Import/Conversions.xlsx
+++ b/matlab/Data_Import/Conversions.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github 2018\Hawkesbury\matlab\Data_Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\matlab\Data_Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BA9D95-03A1-40C2-8304-3A95C0287084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -131,9 +140,6 @@
     <t>WQ_DIAG_TOT_TOC</t>
   </si>
   <si>
-    <t>WQ_DIAG_PHY_TCHA</t>
-  </si>
-  <si>
     <t>ENT</t>
   </si>
   <si>
@@ -180,12 +186,15 @@
   </si>
   <si>
     <t>WQ_SIL_RSI</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_TCHLA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1018,34 +1027,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1056,10 +1065,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1071,10 +1080,10 @@
         <v>31.25</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1085,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1099,10 +1108,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1113,10 +1122,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1127,10 +1136,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1141,10 +1150,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1155,10 +1164,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1170,10 +1179,10 @@
         <v>32.258064516129032</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1185,10 +1194,10 @@
         <v>32.258064516129032</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1200,10 +1209,10 @@
         <v>71.428571428571431</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1215,10 +1224,10 @@
         <v>71.428571428571431</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1230,10 +1239,10 @@
         <v>71.428571428571431</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1245,10 +1254,10 @@
         <v>71.428571428571431</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1260,64 +1269,64 @@
         <v>83.333333333333329</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <f>1000/28.1</f>
         <v>35.587188612099645</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>